<commit_message>
refactors: - extension method for dependency injection - formatting files gitignore
</commit_message>
<xml_diff>
--- a/books.xlsx
+++ b/books.xlsx
@@ -52,7 +52,7 @@
     <x:t>a foundation for computer science</x:t>
   </x:si>
   <x:si>
-    <x:t>Ronald L. Graham; Donald Knuth; Oren PatashnikRonald L. Graham; Donald Knuth; Oren Patashnik</x:t>
+    <x:t>Ronald L. Graham; Donald Knuth; Oren Patashnik</x:t>
   </x:si>
   <x:si>
     <x:t>657</x:t>
@@ -73,7 +73,7 @@
     <x:t>189 Programming Questions and Solutions</x:t>
   </x:si>
   <x:si>
-    <x:t>Gayle Laakmann McDowellGayle Laakmann McDowell</x:t>
+    <x:t>Gayle Laakmann McDowell</x:t>
   </x:si>
   <x:si>
     <x:t>N/A</x:t>
@@ -91,7 +91,7 @@
     <x:t>the special and general theory</x:t>
   </x:si>
   <x:si>
-    <x:t>Albert EinsteinAlbert Einstein</x:t>
+    <x:t>Albert Einstein</x:t>
   </x:si>
   <x:si>
     <x:t>168</x:t>
@@ -106,7 +106,7 @@
     <x:t>On the Origin of Species</x:t>
   </x:si>
   <x:si>
-    <x:t>Charles DarwinCharles Darwin</x:t>
+    <x:t>Charles Darwin</x:t>
   </x:si>
   <x:si>
     <x:t>520</x:t>
@@ -226,19 +226,19 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellXfs>
@@ -536,7 +536,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:H8"/>
+  <x:dimension ref="A1:H7"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -545,11 +545,11 @@
     <x:col min="1" max="3" width="20.710625" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="27.853482" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="39.424911" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="90.139196" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="45.424911" style="0" customWidth="1"/>
     <x:col min="7" max="8" width="20.710625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:8" ht="30" customHeight="1">
+    <x:row r="1" spans="1:8">
       <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -575,7 +575,7 @@
         <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:8" ht="30" customHeight="1">
+    <x:row r="2" spans="1:8">
       <x:c r="A2" s="2">
         <x:v>1</x:v>
       </x:c>
@@ -601,7 +601,7 @@
         <x:v>14</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:8" ht="30" customHeight="1">
+    <x:row r="3" spans="1:8">
       <x:c r="A3" s="3">
         <x:v>2</x:v>
       </x:c>
@@ -627,7 +627,7 @@
         <x:v>14</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:8" ht="30" customHeight="1">
+    <x:row r="4" spans="1:8">
       <x:c r="A4" s="3">
         <x:v>2</x:v>
       </x:c>
@@ -653,7 +653,7 @@
         <x:v>21</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:8" ht="30" customHeight="1">
+    <x:row r="5" spans="1:8">
       <x:c r="A5" s="4">
         <x:v>3</x:v>
       </x:c>
@@ -679,7 +679,7 @@
         <x:v>21</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:8" ht="30" customHeight="1">
+    <x:row r="6" spans="1:8">
       <x:c r="A6" s="4">
         <x:v>3</x:v>
       </x:c>
@@ -705,7 +705,7 @@
         <x:v>27</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:8" ht="30" customHeight="1">
+    <x:row r="7" spans="1:8">
       <x:c r="A7" s="4">
         <x:v>3</x:v>
       </x:c>
@@ -731,7 +731,6 @@
         <x:v>32</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:8" ht="30" customHeight="1"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>